<commit_message>
Found AUC for all cells
Refined the end of the first phase of the 11mM stimulus for all cells, with and without inhibitor.
</commit_message>
<xml_diff>
--- a/Refined_Program/Data/rep3_md.xlsx
+++ b/Refined_Program/Data/rep3_md.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniemorrall/Documents/FarnsworthFall23/11_02_23(Calcium Data Anylsis)/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanie/Documents/GitHub/Calucium-Analysis/Refined_Program/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65281BD-8315-7544-B2DE-351AA9D3850B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2690A45-2CD4-EE45-B86A-FF0984A8F295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17680" yWindow="500" windowWidth="25700" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Treatment</t>
   </si>
@@ -78,6 +78,39 @@
   </si>
   <si>
     <t>2.5wt% RTG NoInh - Islet 4</t>
+  </si>
+  <si>
+    <t>NoRTG Inh - Islet 1</t>
+  </si>
+  <si>
+    <t>NoRTG Inh - Islet 2</t>
+  </si>
+  <si>
+    <t>NoRTG Inh - Islet 3</t>
+  </si>
+  <si>
+    <t>2.5wt% RTG Inh - Islet 1</t>
+  </si>
+  <si>
+    <t>2.5wt% RTG Inh - Islet 2</t>
+  </si>
+  <si>
+    <t>2.5wt% RTG Inh - Islet 3</t>
+  </si>
+  <si>
+    <t>5wt% RTG Inh - Islet 1</t>
+  </si>
+  <si>
+    <t>5wt% RTG Inh - Islet 2</t>
+  </si>
+  <si>
+    <t>5wt% RTG Inh - Islet 3</t>
+  </si>
+  <si>
+    <t>10wt% RTG Inh - Islet 1</t>
+  </si>
+  <si>
+    <t>10wt% RTG Inh - Islet 2</t>
   </si>
 </sst>
 </file>
@@ -87,6 +120,13 @@
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -114,12 +154,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FFD4D4D4"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -171,20 +205,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -520,16 +553,16 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>240</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1860</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2940</v>
       </c>
       <c r="E2">
@@ -537,16 +570,16 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>300</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1500</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>2640</v>
       </c>
       <c r="E3">
@@ -554,16 +587,16 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1440</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2400</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>2940</v>
       </c>
       <c r="E4">
@@ -571,16 +604,16 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>1440</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>2460</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>3180</v>
       </c>
       <c r="E5">
@@ -590,16 +623,16 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>1440</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>2400</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>3180</v>
       </c>
       <c r="E6">
@@ -609,58 +642,56 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>1440</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>2580</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>3180</v>
       </c>
       <c r="E7">
         <v>1595</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="M7" s="6"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>1080</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2280</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>3000</v>
       </c>
       <c r="E8">
         <v>1270</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="M8" s="6"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>1020</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>2280</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>3000</v>
       </c>
       <c r="E9">
@@ -668,21 +699,20 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="6"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>240</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1620</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>2340</v>
       </c>
       <c r="E10">
@@ -690,21 +720,20 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="6"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>240</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>1380</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>2340</v>
       </c>
       <c r="E11">
@@ -712,86 +741,200 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="6"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>180</v>
+      </c>
+      <c r="C12">
+        <v>1500</v>
+      </c>
+      <c r="D12">
+        <v>2700</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="6"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>180</v>
+      </c>
+      <c r="C13">
+        <v>1260</v>
+      </c>
+      <c r="D13">
+        <v>2100</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="6"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>180</v>
+      </c>
+      <c r="C14">
+        <v>1200</v>
+      </c>
+      <c r="D14">
+        <v>2100</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="6"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>900</v>
+      </c>
+      <c r="C15">
+        <v>2160</v>
+      </c>
+      <c r="D15">
+        <v>3000</v>
+      </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="6"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>900</v>
+      </c>
+      <c r="C16">
+        <v>2160</v>
+      </c>
+      <c r="D16">
+        <v>3000</v>
+      </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="6"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>900</v>
+      </c>
+      <c r="C17">
+        <v>2160</v>
+      </c>
+      <c r="D17">
+        <v>3000</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>180</v>
+      </c>
+      <c r="C18">
+        <v>900</v>
+      </c>
+      <c r="D18">
+        <v>2220</v>
+      </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>180</v>
+      </c>
+      <c r="C19">
+        <v>900</v>
+      </c>
+      <c r="D19">
+        <v>2220</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>120</v>
+      </c>
+      <c r="C20">
+        <v>900</v>
+      </c>
+      <c r="D20">
+        <v>2220</v>
+      </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>120</v>
+      </c>
+      <c r="C21">
+        <v>1200</v>
+      </c>
+      <c r="D21">
+        <v>2340</v>
+      </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>120</v>
+      </c>
+      <c r="C22">
+        <v>1200</v>
+      </c>
+      <c r="D22">
+        <v>2400</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
@@ -800,81 +943,81 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" spans="10:14" x14ac:dyDescent="0.2">
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
     </row>
     <row r="34" spans="10:14" x14ac:dyDescent="0.2">
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
     </row>
     <row r="48" spans="10:14" x14ac:dyDescent="0.2">
       <c r="L48" s="2"/>
@@ -925,7 +1068,7 @@
       <c r="L93" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>